<commit_message>
aggiornamento scostamenti A e C
</commit_message>
<xml_diff>
--- a/result/Scostamenti_VenditeC.xlsx
+++ b/result/Scostamenti_VenditeC.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+  <si>
+    <t>CodCliente</t>
+  </si>
   <si>
     <t>QRiscalate</t>
   </si>
@@ -39,6 +42,84 @@
   </si>
   <si>
     <t>Consuntivo</t>
+  </si>
+  <si>
+    <t>C00001</t>
+  </si>
+  <si>
+    <t>C00003</t>
+  </si>
+  <si>
+    <t>C00004</t>
+  </si>
+  <si>
+    <t>C00015</t>
+  </si>
+  <si>
+    <t>C00017</t>
+  </si>
+  <si>
+    <t>C00018</t>
+  </si>
+  <si>
+    <t>C00020</t>
+  </si>
+  <si>
+    <t>C00026</t>
+  </si>
+  <si>
+    <t>C00084</t>
+  </si>
+  <si>
+    <t>C00094</t>
+  </si>
+  <si>
+    <t>C00117</t>
+  </si>
+  <si>
+    <t>C00127</t>
+  </si>
+  <si>
+    <t>C00140</t>
+  </si>
+  <si>
+    <t>C00158</t>
+  </si>
+  <si>
+    <t>C00236</t>
+  </si>
+  <si>
+    <t>C00297</t>
+  </si>
+  <si>
+    <t>C00344</t>
+  </si>
+  <si>
+    <t>C00455</t>
+  </si>
+  <si>
+    <t>C00456</t>
+  </si>
+  <si>
+    <t>C00458</t>
+  </si>
+  <si>
+    <t>C00461</t>
+  </si>
+  <si>
+    <t>C00465</t>
+  </si>
+  <si>
+    <t>C00471</t>
+  </si>
+  <si>
+    <t>C00473</t>
+  </si>
+  <si>
+    <t>C00474</t>
+  </si>
+  <si>
+    <t>C00479</t>
   </si>
 </sst>
 </file>
@@ -387,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -395,7 +476,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,335 +501,371 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="n">
         <v>107.1853543743079</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>5248</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>-1529.213732004429</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>6777.213732004429</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>2540.876382606839</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>4236.337349397591</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>-17.66265060240949</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>4254</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="n">
         <v>19.37084717607974</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>1570</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>-457.4820044296791</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>2027.482004429679</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>-65.85132890365435</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>2093.333333333333</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>-2086.666666666667</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>4180</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="n">
         <v>2135.958748615726</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>34739.3</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>-10122.67808693246</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>44861.97808693246</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>5943.040420668854</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>38918.93766626361</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>-10068.06233373639</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>48987</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="n">
         <v>51.65559246954597</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>122</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>-35.54955703211519</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>157.5495570321152</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>-2004.900442967885</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>2162.45</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>597.8499999999999</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>1564.6</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="n">
         <v>2.582779623477298</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>250</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>-72.84745293466221</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>322.8474529346622</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>-177.1525470653378</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>500</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>380</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="n">
         <v>6.456949058693246</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>530</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>-154.436600221484</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>684.436600221484</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>-103831.5633997785</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>104516</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>51901</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>52615</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="n">
         <v>25.82779623477298</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>4400</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>-1282.115171650056</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>5682.115171650056</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>-62957.88482834995</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>68640</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>61597</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>7043</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="n">
         <v>530.7612126245847</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>19252</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>-5609.836655592466</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>24861.83665559247</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>21301.85612031266</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>3559.980535279805</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>1584.460535279805</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>1975.52</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="n">
         <v>25.82779623477298</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>274</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>-79.84080841638985</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>353.8408084163898</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>271.6408084163899</v>
-      </c>
-      <c r="G10" t="n">
-        <v>82.19999999999999</v>
       </c>
       <c r="H10" t="n">
         <v>82.19999999999999</v>
       </c>
       <c r="I10" t="n">
+        <v>82.19999999999999</v>
+      </c>
+      <c r="J10" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="n">
         <v>1057.648255813953</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>16986.78</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>-4949.774626245846</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>21936.55462624584</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>-66191.44075836951</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>88127.99538461537</v>
       </c>
-      <c r="H11" t="n">
-        <v>-393379.3146153853</v>
-      </c>
       <c r="I11" t="n">
-        <v>481507.3100000007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>-393379.314615385</v>
+      </c>
+      <c r="J11" t="n">
+        <v>481507.3100000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="n">
         <v>11.62250830564784</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>338</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>-98.48975636766329</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>436.4897563676633</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>398.9342008121077</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>37.55555555555556</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>-112.4444444444444</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="n">
         <v>23.24501661129568</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -763,415 +880,460 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
         <v>-17413</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>17413</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="n">
         <v>4660.625830564784</v>
       </c>
-      <c r="C14" t="n">
-        <v>357703.8300000001</v>
-      </c>
       <c r="D14" t="n">
-        <v>-104231.2516818938</v>
+        <v>357703.8300000005</v>
       </c>
       <c r="E14" t="n">
-        <v>461935.0816818939</v>
+        <v>-104231.2516818939</v>
       </c>
       <c r="F14" t="n">
-        <v>461637.7385148116</v>
+        <v>461935.0816818944</v>
       </c>
       <c r="G14" t="n">
-        <v>297.3431670822944</v>
+        <v>461637.7385148121</v>
       </c>
       <c r="H14" t="n">
-        <v>157.3431670822944</v>
+        <v>297.3431670822947</v>
       </c>
       <c r="I14" t="n">
+        <v>157.3431670822947</v>
+      </c>
+      <c r="J14" t="n">
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="n">
         <v>82.64894795127353</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>320</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>-93.24473975636761</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>413.2447397563676</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>293.2447397563676</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>120</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>-812</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>932</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="n">
         <v>1.291389811738649</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>2100</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>-611.9186046511627</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>2711.918604651163</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>-39288.08139534884</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>42000</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>41916</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="n">
         <v>46.49003322259136</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>10550</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>-3074.162513842744</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>13624.16251384274</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>12158.88473606497</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>1465.277777777778</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>850.2777777777778</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>615</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="n">
         <v>3.874169435215947</v>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>490</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>-142.7810077519381</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>632.7810077519381</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>-16843.88565891473</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>17476.66666666667</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>12827.92666666667</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>4648.74</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="n">
         <v>28.41057585825028</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>508</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>-148.0260243632337</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>656.0260243632337</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>-9873.428521091311</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>10529.45454545454</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>-31071.54545454546</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>41601</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="n">
         <v>67.15227021040974</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>2212</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>-644.5542635658912</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>2856.554263565891</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>-1609.984197972571</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>4466.538461538462</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>1962.538461538462</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>2504</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="n">
         <v>20.66223698781838</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>500</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>-145.6949058693244</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>645.6949058693244</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>583.1949058693244</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>62.5</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>-52.5</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="n">
         <v>2.582779623477298</v>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>95</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>-27.68203211517164</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>122.6820321151716</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>75.18203211517164</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>47.5</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>-1502.5</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>1550</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="n">
         <v>1.291389811738649</v>
       </c>
-      <c r="C23" t="n">
+      <c r="D23" t="n">
         <v>320</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>-93.24473975636761</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>413.2447397563676</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>-2146.755260243633</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>2560</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>2480</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="n">
         <v>259.5693521594685</v>
       </c>
-      <c r="C24" t="n">
+      <c r="D24" t="n">
         <v>15066.04</v>
       </c>
-      <c r="D24" t="n">
-        <v>-4390.090559246957</v>
-      </c>
       <c r="E24" t="n">
-        <v>19456.13055924696</v>
+        <v>-4390.090559246955</v>
       </c>
       <c r="F24" t="n">
+        <v>19456.13055924695</v>
+      </c>
+      <c r="G24" t="n">
         <v>19306.21971347581</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>149.9108457711443</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>-1738.589154228856</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>1888.5</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="n">
         <v>103.3111849390919</v>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>1661</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>-483.998477297896</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>2144.998477297896</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>2020.423477297896</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>124.575</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>-235.425</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>360</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="n">
         <v>51.65559246954597</v>
       </c>
-      <c r="C26" t="n">
+      <c r="D26" t="n">
         <v>2100</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>-611.9186046511632</v>
       </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>2711.918604651163</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>2449.418604651163</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>262.5</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>62.5</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="n">
         <v>1.291389811738649</v>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="n">
         <v>20</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>-5.827796234772975</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>25.82779623477298</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>-5094.172203765227</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>5120</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>4467.2</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>652.8</v>
       </c>
     </row>

</xml_diff>